<commit_message>
TP notes update before metting
</commit_message>
<xml_diff>
--- a/notes/try_tp.xlsx
+++ b/notes/try_tp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Desktop\mul_doc\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB37FA1-12A1-43CA-BD64-88619E54E770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675CA030-E689-4636-B7B1-E5A4DCE96001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22740" yWindow="8970" windowWidth="13875" windowHeight="11310" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18855" yWindow="2280" windowWidth="12330" windowHeight="16920" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="try_tp_dec" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Description</t>
   </si>
@@ -208,7 +208,10 @@
     <t>From version control</t>
   </si>
   <si>
-    <t>UPR does not seem right</t>
+    <t>UPR does not seem right; NWP might be wrong</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -216,7 +219,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -311,16 +314,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +388,18 @@
       <sheetName val="Deferrals"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0">
+        <row r="17">
+          <cell r="H17">
+            <v>3291.1138200000023</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="H20">
+            <v>4361.5666600000004</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="1">
         <row r="63">
           <cell r="C63">
@@ -403,7 +417,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1132,7 +1146,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1152,12 +1166,8 @@
       <c r="B1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -1167,71 +1177,63 @@
         <f>'[3]S2 Balance Sheet Summary'!$E$32</f>
         <v>933589.79950986418</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="11">
-        <f>'[3]S2 Balance Sheet Summary'!$E$32</f>
-        <v>933589.79950986418</v>
-      </c>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="B3" s="11">
+        <f>[2]PL!$H$20</f>
+        <v>4361.5666600000004</v>
+      </c>
+      <c r="C3" s="11">
         <v>29911446.990000002</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="B4" s="11">
+        <f>1000*[2]PL!$H$17</f>
+        <v>3291113.8200000022</v>
+      </c>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="B5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="D8" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>